<commit_message>
for(String i : thyoridList) {
</commit_message>
<xml_diff>
--- a/src/je/panse/doro/aeternum/dataxlsx/Sympt12List1.xlsx
+++ b/src/je/panse/doro/aeternum/dataxlsx/Sympt12List1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,162 +21,147 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
-  <si>
-    <t xml:space="preserve">DM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thyroid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URI UTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abodominal pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atypical chest pain</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+  <si>
+    <t xml:space="preserve">increased thirst and urination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increased hunger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fatigue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blurred vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numbness or tingling in the feet or hands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sores that do not heal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexplained weight loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexplained weight gain</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">increased thirst and urination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rapid heartbeat (palpitations)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">body aches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fever</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain in the center of the chest 
-that can feel like pressure, fullness, or squeezing 
-That lasts more than a few minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Where it’s located</t>
-  </si>
-  <si>
-    <t xml:space="preserve">increased hunger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feeling shaky and/or nervous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">headache</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloody stool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain moving from the chest 
-To shoulders, arms, back, or jaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How intense it is</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fatigue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nausea and vomiting that doesn’t resolve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shortness of breath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether it’s dull, stabbing, burning, or cramping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blurred vision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increased appetite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sputum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nausea and vomiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether it comes and goes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numbness or tingling in the feet or hands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diarrhea and more frequent bowel movements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nasal congestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellowish skin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you experience or notice it most</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sores that do not heal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vision changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sneezing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abdomen very tender to touch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feeling faint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether it radiates outward to other areas of your body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unexplained weight loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thin, warm and moist skin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sore throat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swollen abdomen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How long you’ve had it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unexplained weight gain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menstrual changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whether any activities or actions seem to make it worse or better</t>
   </si>
   <si>
     <t xml:space="preserve">• Periarthritis shoulder – Pain and limitation of movements 
 • Cheiroarthropathy – Stiffness and limited mobility of fingers 
 • Neuroarthropathy • Painless unilateral swelling of foot and ankle 
 • Spinal hyperostosis – Mild back pain with preservation of back movements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapid heartbeat (palpitations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">body aches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain in the center of the chest 
+that can feel like pressure, fullness, or squeezing 
+That lasts more than a few minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where it’s located</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling shaky and/or nervous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">headache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloody stool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain moving from the chest 
+To shoulders, arms, back, or jaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How intense it is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nausea and vomiting that doesn’t resolve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shortness of breath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether it’s dull, stabbing, burning, or cramping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increased appetite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sputum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nausea and vomiting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether it comes and goes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diarrhea and more frequent bowel movements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nasal congestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellowish skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you experience or notice it most</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vision changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneezing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdomen very tender to touch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling faint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether it radiates outward to other areas of your body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin, warm and moist skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sore throat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swollen abdomen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How long you’ve had it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menstrual changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether any activities or actions seem to make it worse or better</t>
   </si>
   <si>
     <t xml:space="preserve">Intolerance to heat and excessive sweating</t>
@@ -261,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK KR"/>
@@ -282,13 +267,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK KR"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -333,17 +311,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -367,60 +337,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="32.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="32.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="39.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -441,75 +416,75 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="36.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>25</v>
@@ -518,7 +493,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>27</v>
@@ -529,226 +504,226 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="E7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>49</v>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>